<commit_message>
Updated EWS000003 Traceability Matrix Easy WiFi Setup UX - changed.xlsx
</commit_message>
<xml_diff>
--- a/Documents/External/EWS000003 Traceability Matrix Easy WiFi Setup UX - changed.xlsx
+++ b/Documents/External/EWS000003 Traceability Matrix Easy WiFi Setup UX - changed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynnslooten/Documents/Projects/Philips EWS/QMS documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynnslooten/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="887" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="887"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1440" windowHeight="647" tabRatio="887" activeSheetId="2"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1440" windowHeight="647" tabRatio="887" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -156,6 +156,321 @@
     <t>Verification Report Android</t>
   </si>
   <si>
+    <t>DRS Requirement ID</t>
+  </si>
+  <si>
+    <t>DRS Title</t>
+  </si>
+  <si>
+    <t>Verification Test ID</t>
+  </si>
+  <si>
+    <t>Verification Test Title</t>
+  </si>
+  <si>
+    <t>86161</t>
+  </si>
+  <si>
+    <t>The component shall support iOS 11.</t>
+  </si>
+  <si>
+    <t>71328</t>
+  </si>
+  <si>
+    <t>The user connects the device using EWS</t>
+  </si>
+  <si>
+    <t>71329</t>
+  </si>
+  <si>
+    <t>The Users phone is not connected to WiFi</t>
+  </si>
+  <si>
+    <t>71331</t>
+  </si>
+  <si>
+    <t>The users phone is not connected to the network onto which they want to setup the device</t>
+  </si>
+  <si>
+    <t>71332</t>
+  </si>
+  <si>
+    <t>The user gets a trouble shoot page to help connect the device</t>
+  </si>
+  <si>
+    <t>71335</t>
+  </si>
+  <si>
+    <t>The user gets a trouble shoot page to help connect access point</t>
+  </si>
+  <si>
+    <t>71342</t>
+  </si>
+  <si>
+    <t>The users phone can not connect to Philips Setup</t>
+  </si>
+  <si>
+    <t>71357</t>
+  </si>
+  <si>
+    <t>The user enters an incorrect WiFi password</t>
+  </si>
+  <si>
+    <t>76994</t>
+  </si>
+  <si>
+    <t>Cancel flow during setup of device</t>
+  </si>
+  <si>
+    <t>77006</t>
+  </si>
+  <si>
+    <t>Cancel flow during troubleshooting</t>
+  </si>
+  <si>
+    <t>77026</t>
+  </si>
+  <si>
+    <t>The user decides not to cancel the flow</t>
+  </si>
+  <si>
+    <t>86194</t>
+  </si>
+  <si>
+    <t>The component shall support Android Oreo.</t>
+  </si>
+  <si>
+    <t>93480</t>
+  </si>
+  <si>
+    <t>The component shall support iOS 10.</t>
+  </si>
+  <si>
+    <t>93481</t>
+  </si>
+  <si>
+    <t>The component shall support iOS 9.</t>
+  </si>
+  <si>
+    <t>93482</t>
+  </si>
+  <si>
+    <t>The component shall support Android Marshmallow.</t>
+  </si>
+  <si>
+    <t>93483</t>
+  </si>
+  <si>
+    <t>The component shall support Android Nougat.</t>
+  </si>
+  <si>
+    <t>93484</t>
+  </si>
+  <si>
+    <t>The component shall support Android Lollipop.</t>
+  </si>
+  <si>
+    <t>70300</t>
+  </si>
+  <si>
+    <t>The component shall be able to connect an appliance to the Wi-Fi network specified by the user.</t>
+  </si>
+  <si>
+    <t>The component must be DLS compliant.</t>
+  </si>
+  <si>
+    <t>70308</t>
+  </si>
+  <si>
+    <t>The component shall aid the user to put his appliance into setup mode.</t>
+  </si>
+  <si>
+    <t>70309</t>
+  </si>
+  <si>
+    <t>The component shall aid the user when the appliance can not be found on his home network after the passphrase has been set on the appliance.</t>
+  </si>
+  <si>
+    <t>71362</t>
+  </si>
+  <si>
+    <t>The users phone connects to incorrect WiFi network</t>
+  </si>
+  <si>
+    <t>70310</t>
+  </si>
+  <si>
+    <t>The component shall aid the user to switch between setup and home wifi networks.</t>
+  </si>
+  <si>
+    <t>70311</t>
+  </si>
+  <si>
+    <t>The component shall tell the user when appliance is correctly configured with the home network.</t>
+  </si>
+  <si>
+    <t>70312</t>
+  </si>
+  <si>
+    <t>The component shall dismiss all screens after a successful setup.</t>
+  </si>
+  <si>
+    <t>94957</t>
+  </si>
+  <si>
+    <t>The user can return to EWSDemoApp after EWS flow has been performed</t>
+  </si>
+  <si>
+    <t>70313</t>
+  </si>
+  <si>
+    <t>The flow and design of the component shall be implemented according to the design book version PI17.4.S4.</t>
+  </si>
+  <si>
+    <t>77210</t>
+  </si>
+  <si>
+    <t>Connect device with an unsecured network</t>
+  </si>
+  <si>
+    <t>77230</t>
+  </si>
+  <si>
+    <t>The users phone is connected with 4G/3G</t>
+  </si>
+  <si>
+    <t>72728</t>
+  </si>
+  <si>
+    <t>The component shall be available in English.</t>
+  </si>
+  <si>
+    <t>93899</t>
+  </si>
+  <si>
+    <t>EWS Happy Flow in English language</t>
+  </si>
+  <si>
+    <t>93900</t>
+  </si>
+  <si>
+    <t>EWS unHappy Flow in English language</t>
+  </si>
+  <si>
+    <t>72729</t>
+  </si>
+  <si>
+    <t>The component shall be available in German.</t>
+  </si>
+  <si>
+    <t>93873</t>
+  </si>
+  <si>
+    <t>EWS Happy Flow in German language</t>
+  </si>
+  <si>
+    <t>93874</t>
+  </si>
+  <si>
+    <t>EWS unHappy Flow in German language</t>
+  </si>
+  <si>
+    <t>72730</t>
+  </si>
+  <si>
+    <t>The component shall be available in Simplified Chinese.</t>
+  </si>
+  <si>
+    <t>93884</t>
+  </si>
+  <si>
+    <t>EWS Happy Flow in Simplified Chinese language</t>
+  </si>
+  <si>
+    <t>93897</t>
+  </si>
+  <si>
+    <t>EWS unHappy Flow in Simplified Chinese language</t>
+  </si>
+  <si>
+    <t>72732</t>
+  </si>
+  <si>
+    <t>The component shall be available in Traditional Chinese.</t>
+  </si>
+  <si>
+    <t>93872</t>
+  </si>
+  <si>
+    <t>EWS Happy Flow in Traditional Chinese language</t>
+  </si>
+  <si>
+    <t>93875</t>
+  </si>
+  <si>
+    <t>EWS unHappy Flow in Traditional Chinese language</t>
+  </si>
+  <si>
+    <t>70304</t>
+  </si>
+  <si>
+    <t>The component must be customizable for different products.</t>
+  </si>
+  <si>
+    <t>94953</t>
+  </si>
+  <si>
+    <t>The user can select customised product in EWSDemoApp and perform EWS flow</t>
+  </si>
+  <si>
+    <t>70306</t>
+  </si>
+  <si>
+    <t>The component shall implement the uApp interface, so that it can be integrated into applications.</t>
+  </si>
+  <si>
+    <t>94936</t>
+  </si>
+  <si>
+    <t>The user can perform EWS flow from Reference App</t>
+  </si>
+  <si>
+    <t>71552</t>
+  </si>
+  <si>
+    <t>The component must instruct CommLib to accept the first mismatched pin for a device it encounters during setup mode.</t>
+  </si>
+  <si>
+    <t>72609</t>
+  </si>
+  <si>
+    <t>CommLib accepts first mismatched pin it encounters during setup mode</t>
+  </si>
+  <si>
+    <t>86089</t>
+  </si>
+  <si>
+    <t>The component shall provide analytics tagging.</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>Lynn Slooten</t>
+  </si>
+  <si>
+    <t>Initial Draft</t>
+  </si>
+  <si>
+    <t>Thijs Winter</t>
+  </si>
+  <si>
+    <t>Group Leader</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -163,7 +478,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>This Requirement Traceability Matrix is applicable for the work done in release PI 17.5.</t>
+      <t>This Requirement Traceability Matrix is applicable for the work done in Platform Release 2017.5.0.</t>
     </r>
     <r>
       <rPr>
@@ -175,321 +490,6 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-  </si>
-  <si>
-    <t>DRS Requirement ID</t>
-  </si>
-  <si>
-    <t>DRS Title</t>
-  </si>
-  <si>
-    <t>Verification Test ID</t>
-  </si>
-  <si>
-    <t>Verification Test Title</t>
-  </si>
-  <si>
-    <t>86161</t>
-  </si>
-  <si>
-    <t>The component shall support iOS 11.</t>
-  </si>
-  <si>
-    <t>71328</t>
-  </si>
-  <si>
-    <t>The user connects the device using EWS</t>
-  </si>
-  <si>
-    <t>71329</t>
-  </si>
-  <si>
-    <t>The Users phone is not connected to WiFi</t>
-  </si>
-  <si>
-    <t>71331</t>
-  </si>
-  <si>
-    <t>The users phone is not connected to the network onto which they want to setup the device</t>
-  </si>
-  <si>
-    <t>71332</t>
-  </si>
-  <si>
-    <t>The user gets a trouble shoot page to help connect the device</t>
-  </si>
-  <si>
-    <t>71335</t>
-  </si>
-  <si>
-    <t>The user gets a trouble shoot page to help connect access point</t>
-  </si>
-  <si>
-    <t>71342</t>
-  </si>
-  <si>
-    <t>The users phone can not connect to Philips Setup</t>
-  </si>
-  <si>
-    <t>71357</t>
-  </si>
-  <si>
-    <t>The user enters an incorrect WiFi password</t>
-  </si>
-  <si>
-    <t>76994</t>
-  </si>
-  <si>
-    <t>Cancel flow during setup of device</t>
-  </si>
-  <si>
-    <t>77006</t>
-  </si>
-  <si>
-    <t>Cancel flow during troubleshooting</t>
-  </si>
-  <si>
-    <t>77026</t>
-  </si>
-  <si>
-    <t>The user decides not to cancel the flow</t>
-  </si>
-  <si>
-    <t>86194</t>
-  </si>
-  <si>
-    <t>The component shall support Android Oreo.</t>
-  </si>
-  <si>
-    <t>93480</t>
-  </si>
-  <si>
-    <t>The component shall support iOS 10.</t>
-  </si>
-  <si>
-    <t>93481</t>
-  </si>
-  <si>
-    <t>The component shall support iOS 9.</t>
-  </si>
-  <si>
-    <t>93482</t>
-  </si>
-  <si>
-    <t>The component shall support Android Marshmallow.</t>
-  </si>
-  <si>
-    <t>93483</t>
-  </si>
-  <si>
-    <t>The component shall support Android Nougat.</t>
-  </si>
-  <si>
-    <t>93484</t>
-  </si>
-  <si>
-    <t>The component shall support Android Lollipop.</t>
-  </si>
-  <si>
-    <t>70300</t>
-  </si>
-  <si>
-    <t>The component shall be able to connect an appliance to the Wi-Fi network specified by the user.</t>
-  </si>
-  <si>
-    <t>The component must be DLS compliant.</t>
-  </si>
-  <si>
-    <t>70308</t>
-  </si>
-  <si>
-    <t>The component shall aid the user to put his appliance into setup mode.</t>
-  </si>
-  <si>
-    <t>70309</t>
-  </si>
-  <si>
-    <t>The component shall aid the user when the appliance can not be found on his home network after the passphrase has been set on the appliance.</t>
-  </si>
-  <si>
-    <t>71362</t>
-  </si>
-  <si>
-    <t>The users phone connects to incorrect WiFi network</t>
-  </si>
-  <si>
-    <t>70310</t>
-  </si>
-  <si>
-    <t>The component shall aid the user to switch between setup and home wifi networks.</t>
-  </si>
-  <si>
-    <t>70311</t>
-  </si>
-  <si>
-    <t>The component shall tell the user when appliance is correctly configured with the home network.</t>
-  </si>
-  <si>
-    <t>70312</t>
-  </si>
-  <si>
-    <t>The component shall dismiss all screens after a successful setup.</t>
-  </si>
-  <si>
-    <t>94957</t>
-  </si>
-  <si>
-    <t>The user can return to EWSDemoApp after EWS flow has been performed</t>
-  </si>
-  <si>
-    <t>70313</t>
-  </si>
-  <si>
-    <t>The flow and design of the component shall be implemented according to the design book version PI17.4.S4.</t>
-  </si>
-  <si>
-    <t>77210</t>
-  </si>
-  <si>
-    <t>Connect device with an unsecured network</t>
-  </si>
-  <si>
-    <t>77230</t>
-  </si>
-  <si>
-    <t>The users phone is connected with 4G/3G</t>
-  </si>
-  <si>
-    <t>72728</t>
-  </si>
-  <si>
-    <t>The component shall be available in English.</t>
-  </si>
-  <si>
-    <t>93899</t>
-  </si>
-  <si>
-    <t>EWS Happy Flow in English language</t>
-  </si>
-  <si>
-    <t>93900</t>
-  </si>
-  <si>
-    <t>EWS unHappy Flow in English language</t>
-  </si>
-  <si>
-    <t>72729</t>
-  </si>
-  <si>
-    <t>The component shall be available in German.</t>
-  </si>
-  <si>
-    <t>93873</t>
-  </si>
-  <si>
-    <t>EWS Happy Flow in German language</t>
-  </si>
-  <si>
-    <t>93874</t>
-  </si>
-  <si>
-    <t>EWS unHappy Flow in German language</t>
-  </si>
-  <si>
-    <t>72730</t>
-  </si>
-  <si>
-    <t>The component shall be available in Simplified Chinese.</t>
-  </si>
-  <si>
-    <t>93884</t>
-  </si>
-  <si>
-    <t>EWS Happy Flow in Simplified Chinese language</t>
-  </si>
-  <si>
-    <t>93897</t>
-  </si>
-  <si>
-    <t>EWS unHappy Flow in Simplified Chinese language</t>
-  </si>
-  <si>
-    <t>72732</t>
-  </si>
-  <si>
-    <t>The component shall be available in Traditional Chinese.</t>
-  </si>
-  <si>
-    <t>93872</t>
-  </si>
-  <si>
-    <t>EWS Happy Flow in Traditional Chinese language</t>
-  </si>
-  <si>
-    <t>93875</t>
-  </si>
-  <si>
-    <t>EWS unHappy Flow in Traditional Chinese language</t>
-  </si>
-  <si>
-    <t>70304</t>
-  </si>
-  <si>
-    <t>The component must be customizable for different products.</t>
-  </si>
-  <si>
-    <t>94953</t>
-  </si>
-  <si>
-    <t>The user can select customised product in EWSDemoApp and perform EWS flow</t>
-  </si>
-  <si>
-    <t>70306</t>
-  </si>
-  <si>
-    <t>The component shall implement the uApp interface, so that it can be integrated into applications.</t>
-  </si>
-  <si>
-    <t>94936</t>
-  </si>
-  <si>
-    <t>The user can perform EWS flow from Reference App</t>
-  </si>
-  <si>
-    <t>71552</t>
-  </si>
-  <si>
-    <t>The component must instruct CommLib to accept the first mismatched pin for a device it encounters during setup mode.</t>
-  </si>
-  <si>
-    <t>72609</t>
-  </si>
-  <si>
-    <t>CommLib accepts first mismatched pin it encounters during setup mode</t>
-  </si>
-  <si>
-    <t>86089</t>
-  </si>
-  <si>
-    <t>The component shall provide analytics tagging.</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>Lynn Slooten</t>
-  </si>
-  <si>
-    <t>Initial Draft</t>
-  </si>
-  <si>
-    <t>Thijs Winter</t>
-  </si>
-  <si>
-    <t>Group Leader</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -719,17 +719,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -875,7 +875,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{03823957-A7D6-514D-BF89-4CD73B0C21CD}" diskRevisions="1" revisionId="1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A41C3A18-8DEE-BC4C-B029-0D0E49D0418F}" diskRevisions="1" revisionId="2" version="2">
   <header guid="{1A553375-48A2-9244-A11E-9A3320265BCF}" dateTime="2017-11-17T15:09:12" maxSheetId="4" userName="Microsoft Office User" r:id="rId1">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -884,6 +884,13 @@
     </sheetIdMap>
   </header>
   <header guid="{03823957-A7D6-514D-BF89-4CD73B0C21CD}" dateTime="2017-11-17T15:11:18" maxSheetId="4" userName="Microsoft Office User" r:id="rId2" minRId="1">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A41C3A18-8DEE-BC4C-B029-0D0E49D0418F}" dateTime="2017-11-20T13:14:05" maxSheetId="4" userName="Microsoft Office User" r:id="rId3" minRId="2">
     <sheetIdMap count="3">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -967,9 +974,65 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="2" sId="1">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This Requirement Traceability Matrix is applicable for the work done in release PI 17.5.</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color theme="5"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>This Requirement Traceability Matrix is applicable for the work done in Platform Release 2017.5.0.</t>
+        </r>
+        <r>
+          <rPr>
+            <i/>
+            <sz val="11"/>
+            <color theme="5"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" action="delete"/>
+  <rcv guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{03823957-A7D6-514D-BF89-4CD73B0C21CD}" name="Microsoft Office User" id="-296994960" dateTime="2017-11-17T15:21:50"/>
+  <userInfo guid="{A41C3A18-8DEE-BC4C-B029-0D0E49D0418F}" name="Microsoft Office User" id="-296959360" dateTime="2017-11-20T13:13:25"/>
 </users>
 </file>
 
@@ -1263,7 +1326,7 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
@@ -1290,14 +1353,14 @@
       <c r="F1" s="34"/>
     </row>
     <row r="2" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36"/>
@@ -1318,14 +1381,14 @@
       <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
+      <c r="A6" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
@@ -1338,15 +1401,15 @@
       <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="34" t="s">
@@ -1357,9 +1420,9 @@
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="34"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
@@ -1566,16 +1629,16 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
@@ -1596,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A95" zoomScale="169" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView view="pageLayout" topLeftCell="A95" zoomScale="169" zoomScalePageLayoutView="169" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1611,758 +1674,758 @@
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>26</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="C2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="D2" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="29"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="29"/>
       <c r="C6" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>51</v>
-      </c>
       <c r="C12" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="29"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="29"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="29"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="29"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="29"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>53</v>
-      </c>
       <c r="C22" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="29"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="29"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="29" t="s">
-        <v>55</v>
-      </c>
       <c r="C32" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D33" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="29"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="29"/>
       <c r="B36" s="29"/>
       <c r="C36" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="29"/>
       <c r="B37" s="29"/>
       <c r="C37" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="29"/>
       <c r="B38" s="29"/>
       <c r="C38" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="29"/>
       <c r="B39" s="29"/>
       <c r="C39" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D39" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="29"/>
       <c r="B40" s="29"/>
       <c r="C40" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D40" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="29"/>
       <c r="B41" s="29"/>
       <c r="C41" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="29" t="s">
-        <v>57</v>
-      </c>
       <c r="C42" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="29"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D43" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
       <c r="C44" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D44" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D44" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="29"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A46" s="29"/>
       <c r="B46" s="29"/>
       <c r="C46" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D46" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="29"/>
       <c r="B47" s="29"/>
       <c r="C47" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="29"/>
       <c r="B48" s="29"/>
       <c r="C48" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="29"/>
       <c r="B49" s="29"/>
       <c r="C49" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D49" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="29"/>
       <c r="B50" s="29"/>
       <c r="C50" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D50" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="29"/>
       <c r="B51" s="29"/>
       <c r="C51" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="29" t="s">
-        <v>59</v>
-      </c>
       <c r="C52" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D52" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="29"/>
       <c r="B53" s="29"/>
       <c r="C53" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D53" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="29"/>
       <c r="B54" s="29"/>
       <c r="C54" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D54" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="29"/>
       <c r="B55" s="29"/>
       <c r="C55" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D55" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A56" s="29"/>
       <c r="B56" s="29"/>
       <c r="C56" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D56" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="29"/>
       <c r="B57" s="29"/>
       <c r="C57" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="29"/>
       <c r="B58" s="29"/>
       <c r="C58" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="29"/>
       <c r="B59" s="29"/>
       <c r="C59" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="29"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="29"/>
       <c r="B61" s="29"/>
       <c r="C61" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="29" t="s">
-        <v>61</v>
-      </c>
       <c r="C62" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="29"/>
       <c r="B63" s="29"/>
       <c r="C63" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" s="29"/>
       <c r="B64" s="29"/>
       <c r="C64" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="29"/>
       <c r="B65" s="29"/>
       <c r="C65" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A66" s="29"/>
       <c r="B66" s="29"/>
       <c r="C66" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="29"/>
       <c r="B67" s="29"/>
       <c r="C67" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D67" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="29"/>
       <c r="B68" s="29"/>
       <c r="C68" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D68" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="29"/>
       <c r="B69" s="29"/>
       <c r="C69" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D69" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D69" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="29"/>
       <c r="B70" s="29"/>
       <c r="C70" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D70" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D70" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="29"/>
       <c r="B71" s="29"/>
       <c r="C71" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D71" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A72" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B72" s="29" t="s">
-        <v>63</v>
-      </c>
       <c r="C72" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D72" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D72" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.2">
@@ -2370,474 +2433,474 @@
         <v>70307</v>
       </c>
       <c r="B73" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D73" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D73" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="29"/>
       <c r="B74" s="29"/>
       <c r="C74" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D74" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="29"/>
       <c r="B75" s="29"/>
       <c r="C75" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D75" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D75" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" s="29"/>
       <c r="B76" s="29"/>
       <c r="C76" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D76" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="29"/>
       <c r="B77" s="29"/>
       <c r="C77" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D77" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D77" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="29"/>
       <c r="B78" s="29"/>
       <c r="C78" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D78" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="29"/>
       <c r="B79" s="29"/>
       <c r="C79" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D79" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D79" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="29"/>
       <c r="B80" s="29"/>
       <c r="C80" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D80" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D80" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="29"/>
       <c r="B81" s="29"/>
       <c r="C81" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D81" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D81" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="29"/>
       <c r="B82" s="29"/>
       <c r="C82" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D82" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A83" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B83" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B83" s="29" t="s">
-        <v>66</v>
-      </c>
       <c r="C83" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D83" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D83" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="75" x14ac:dyDescent="0.2">
       <c r="A84" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B84" s="29" t="s">
+      <c r="C84" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C84" s="29" t="s">
+      <c r="D84" s="29" t="s">
         <v>69</v>
-      </c>
-      <c r="D84" s="29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A85" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B85" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="B85" s="29" t="s">
-        <v>72</v>
-      </c>
       <c r="C85" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D85" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A86" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B86" s="29" t="s">
-        <v>74</v>
-      </c>
       <c r="C86" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D86" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A87" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B87" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B87" s="29" t="s">
+      <c r="C87" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C87" s="29" t="s">
+      <c r="D87" s="29" t="s">
         <v>77</v>
-      </c>
-      <c r="D87" s="29" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A88" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B88" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B88" s="29" t="s">
-        <v>80</v>
-      </c>
       <c r="C88" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D88" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="29"/>
       <c r="B89" s="29"/>
       <c r="C89" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D89" s="29" t="s">
         <v>32</v>
-      </c>
-      <c r="D89" s="29" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="29"/>
       <c r="B90" s="29"/>
       <c r="C90" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D90" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="D90" s="29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="29"/>
       <c r="B91" s="29"/>
       <c r="C91" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91" s="29" t="s">
         <v>36</v>
-      </c>
-      <c r="D91" s="29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="29"/>
       <c r="B92" s="29"/>
       <c r="C92" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D92" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D92" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="29"/>
       <c r="B93" s="29"/>
       <c r="C93" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D93" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="29"/>
       <c r="B94" s="29"/>
       <c r="C94" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D94" s="29" t="s">
         <v>42</v>
-      </c>
-      <c r="D94" s="29" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="29"/>
       <c r="B95" s="29"/>
       <c r="C95" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D95" s="29" t="s">
         <v>69</v>
-      </c>
-      <c r="D95" s="29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="29"/>
       <c r="B96" s="29"/>
       <c r="C96" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" s="29" t="s">
         <v>44</v>
-      </c>
-      <c r="D96" s="29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="29"/>
       <c r="B97" s="29"/>
       <c r="C97" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D97" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="D97" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="29"/>
       <c r="B98" s="29"/>
       <c r="C98" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D98" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="D98" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="29"/>
       <c r="B99" s="29"/>
       <c r="C99" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D99" s="29" t="s">
         <v>81</v>
-      </c>
-      <c r="D99" s="29" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="29"/>
       <c r="B100" s="29"/>
       <c r="C100" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D100" s="29" t="s">
         <v>83</v>
-      </c>
-      <c r="D100" s="29" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B101" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B101" s="29" t="s">
+      <c r="C101" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C101" s="29" t="s">
+      <c r="D101" s="29" t="s">
         <v>87</v>
-      </c>
-      <c r="D101" s="29" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="29"/>
       <c r="B102" s="29"/>
       <c r="C102" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D102" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="D102" s="29" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A103" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B103" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B103" s="29" t="s">
+      <c r="C103" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C103" s="29" t="s">
+      <c r="D103" s="29" t="s">
         <v>93</v>
-      </c>
-      <c r="D103" s="29" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="29"/>
       <c r="B104" s="29"/>
       <c r="C104" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D104" s="29" t="s">
         <v>95</v>
-      </c>
-      <c r="D104" s="29" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A105" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B105" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B105" s="29" t="s">
+      <c r="C105" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C105" s="29" t="s">
+      <c r="D105" s="29" t="s">
         <v>99</v>
-      </c>
-      <c r="D105" s="29" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="29"/>
       <c r="B106" s="29"/>
       <c r="C106" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="D106" s="29" t="s">
         <v>101</v>
-      </c>
-      <c r="D106" s="29" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A107" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="B107" s="29" t="s">
+      <c r="C107" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="29" t="s">
+      <c r="D107" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="D107" s="29" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="29"/>
       <c r="B108" s="29"/>
       <c r="C108" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="D108" s="29" t="s">
         <v>107</v>
-      </c>
-      <c r="D108" s="29" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A109" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="29" t="s">
+      <c r="C109" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C109" s="29" t="s">
+      <c r="D109" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="D109" s="29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A110" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B110" s="29" t="s">
+      <c r="C110" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="C110" s="29" t="s">
+      <c r="D110" s="29" t="s">
         <v>115</v>
-      </c>
-      <c r="D110" s="29" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="60" x14ac:dyDescent="0.2">
       <c r="A111" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="B111" s="29" t="s">
+      <c r="C111" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="C111" s="29" t="s">
+      <c r="D111" s="29" t="s">
         <v>119</v>
-      </c>
-      <c r="D111" s="29" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A112" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B112" s="29" t="s">
-        <v>122</v>
-      </c>
       <c r="C112" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D112" s="29" t="s">
         <v>30</v>
-      </c>
-      <c r="D112" s="29" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="29"/>
       <c r="B113" s="29"/>
       <c r="C113" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D113" s="29" t="s">
         <v>40</v>
-      </c>
-      <c r="D113" s="29" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" scale="169" view="pageLayout" topLeftCell="A101">
+    <customSheetView guid="{B643A179-4F56-C84F-B243-C8CAAA56860F}" scale="169" view="pageLayout" topLeftCell="A95">
       <selection activeCell="D109" sqref="D109"/>
       <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
       <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2909,19 +2972,19 @@
     </row>
     <row r="4" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="32">
         <v>43055</v>
       </c>
       <c r="C4" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="31" t="s">
-        <v>125</v>
-      </c>
       <c r="E4" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -2969,10 +3032,10 @@
     </row>
     <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>126</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>127</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>

</xml_diff>